<commit_message>
copied No and added Sw landscape data to GRASS db, and updated metadata; created metadata_update functions
</commit_message>
<xml_diff>
--- a/data/spatialdb_metadata_sweden_20211101.xlsx
+++ b/data/spatialdb_metadata_sweden_20211101.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bernardo\00_academico\07_projetos\05_reindeer\05_env_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\41203800_oneimpact\grass-db\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E293B8-647A-4744-B79E-2B3825E97B0C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="213">
   <si>
     <t>Layer name</t>
   </si>
@@ -661,11 +662,53 @@
   <si>
     <t>Sven Adler - SLU</t>
   </si>
+  <si>
+    <t>landcover_smd_25m_2004</t>
+  </si>
+  <si>
+    <t>This is a land cover map for Sweden (Svenska CORINE Marktäckedata - SMD), a map based on LANDSAT TM satellite images and several other products from Lantmæteriet and other Swedish institutions, with 57 land use classes and 25m resolution.</t>
+  </si>
+  <si>
+    <t>CORINE Land Cover | Lantmäteriet (lantmateriet.se)</t>
+  </si>
+  <si>
+    <t>CORINE Land Cover</t>
+  </si>
+  <si>
+    <t>Model of lichen abundance (or probability of occurrence) created based on remote sensing and generalized additive modeling</t>
+  </si>
+  <si>
+    <t>Model of lichen abundance (or probability of occurrence) created based on remote sensing and generalized additive modeling, callibrated for the district of Tåssåsen based on field samples collected in the district</t>
+  </si>
+  <si>
+    <t>Model of lichen abundance (or probability of occurrence) created based on remote sensing and generalized additive modeling, callibrated for the district of Mittådalen based on field samples collected in the district</t>
+  </si>
+  <si>
+    <t>[0, 100]</t>
+  </si>
+  <si>
+    <t>Mittådalen reindeer herding area</t>
+  </si>
+  <si>
+    <t>Tåssåsen reindeer herding area</t>
+  </si>
+  <si>
+    <t>Reindeer herding area in Sweden, with exception of some reindeer herding districts</t>
+  </si>
+  <si>
+    <t>Derived</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>Sven Adler</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -831,7 +874,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Excel Built-in Check Cell" xfId="1"/>
+    <cellStyle name="Excel Built-in Check Cell" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1178,39 +1221,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:TW42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomLeft" activeCell="S42" sqref="A1:S42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.7265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.81640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.54296875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.26953125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="27.81640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="36.453125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7265625" style="1"/>
-    <col min="8" max="8" width="16.1796875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.26953125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.453125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="20.1796875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="16.7265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="39.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="36.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="1"/>
+    <col min="8" max="8" width="16.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" style="1" customWidth="1"/>
     <col min="13" max="14" width="16" style="1" customWidth="1"/>
-    <col min="15" max="15" width="13.81640625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.81640625" style="1" customWidth="1"/>
-    <col min="17" max="18" width="16.7265625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="17.54296875" style="1" customWidth="1"/>
-    <col min="20" max="1023" width="8.7265625" style="1"/>
-    <col min="1024" max="1025" width="11.54296875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="13.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" style="1" customWidth="1"/>
+    <col min="17" max="18" width="16.7109375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="17.5703125" style="1" customWidth="1"/>
+    <col min="20" max="541" width="8.7109375" style="1"/>
+    <col min="542" max="543" width="11.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1269,7 +1312,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="138" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" ht="138" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>165</v>
       </c>
@@ -1328,7 +1371,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="39.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" ht="40.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>166</v>
       </c>
@@ -1385,7 +1428,7 @@
       </c>
       <c r="S3" s="6"/>
     </row>
-    <row r="4" spans="1:19" s="7" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" s="7" customFormat="1" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>34</v>
       </c>
@@ -1439,7 +1482,7 @@
       </c>
       <c r="S4" s="6"/>
     </row>
-    <row r="5" spans="1:19" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" ht="129.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>40</v>
       </c>
@@ -1498,7 +1541,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="26.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" ht="27" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>164</v>
       </c>
@@ -1554,7 +1597,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="7" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" s="7" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>51</v>
       </c>
@@ -1585,7 +1628,7 @@
       <c r="Q7" s="10"/>
       <c r="R7" s="10"/>
     </row>
-    <row r="8" spans="1:19" s="15" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" s="15" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
         <v>168</v>
       </c>
@@ -1641,7 +1684,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:19" s="15" customFormat="1" ht="65" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" s="15" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>175</v>
       </c>
@@ -1697,7 +1740,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:19" s="15" customFormat="1" ht="39" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" s="15" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
         <v>179</v>
       </c>
@@ -1753,7 +1796,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:19" s="7" customFormat="1" ht="39" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" s="7" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>177</v>
       </c>
@@ -1809,7 +1852,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="65.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>54</v>
       </c>
@@ -1865,7 +1908,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="39.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:19" ht="39" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>64</v>
       </c>
@@ -1921,7 +1964,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:19" s="7" customFormat="1" ht="39" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" s="7" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>70</v>
       </c>
@@ -1977,7 +2020,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:19" s="7" customFormat="1" ht="65" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" s="7" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>74</v>
       </c>
@@ -2033,7 +2076,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="78.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>78</v>
       </c>
@@ -2083,7 +2126,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:19" s="7" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:19" s="7" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>82</v>
       </c>
@@ -2107,7 +2150,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="53.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:19" ht="66" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>125</v>
       </c>
@@ -2164,7 +2207,7 @@
       </c>
       <c r="S18" s="12"/>
     </row>
-    <row r="19" spans="1:19" s="7" customFormat="1" ht="53.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:19" s="7" customFormat="1" ht="66" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>132</v>
       </c>
@@ -2221,9 +2264,9 @@
       </c>
       <c r="S19" s="12"/>
     </row>
-    <row r="20" spans="1:19" s="7" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:19" s="7" customFormat="1" ht="103.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>55</v>
@@ -2232,29 +2275,55 @@
         <v>56</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>197</v>
+        <v>126</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="F20" s="5"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
+        <v>46</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J20" s="1">
+        <v>2004</v>
+      </c>
+      <c r="K20" s="1">
+        <v>25</v>
+      </c>
+      <c r="L20" s="1">
+        <v>25</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P20" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="S20" s="12"/>
     </row>
-    <row r="21" spans="1:19" s="7" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:19" s="7" customFormat="1" ht="78.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>55</v>
@@ -2268,24 +2337,46 @@
       <c r="E21" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="F21" s="5"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
+      <c r="F21" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K21" s="1">
+        <v>10</v>
+      </c>
+      <c r="L21" s="1">
+        <v>10</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>211</v>
+      </c>
       <c r="P21" s="14"/>
       <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
+      <c r="R21" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="S21" s="12"/>
     </row>
-    <row r="22" spans="1:19" s="7" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:19" s="7" customFormat="1" ht="78.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>55</v>
@@ -2299,24 +2390,46 @@
       <c r="E22" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="F22" s="5"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
+      <c r="F22" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K22" s="1">
+        <v>10</v>
+      </c>
+      <c r="L22" s="1">
+        <v>10</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>211</v>
+      </c>
       <c r="P22" s="14"/>
       <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
+      <c r="R22" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="S22" s="12"/>
     </row>
-    <row r="23" spans="1:19" s="7" customFormat="1" ht="92.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:19" s="7" customFormat="1" ht="40.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>55</v>
@@ -2325,55 +2438,51 @@
         <v>56</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>183</v>
+        <v>203</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>24</v>
+        <v>206</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>24</v>
+        <v>24</v>
+      </c>
+      <c r="K23" s="1">
+        <v>10</v>
+      </c>
+      <c r="L23" s="1">
+        <v>10</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>26</v>
+        <v>209</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>27</v>
+        <v>210</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P23" s="14" t="s">
-        <v>187</v>
-      </c>
-      <c r="Q23" s="1" t="s">
-        <v>188</v>
-      </c>
+        <v>211</v>
+      </c>
+      <c r="P23" s="14"/>
+      <c r="Q23" s="1"/>
       <c r="R23" s="1" t="s">
-        <v>30</v>
+        <v>212</v>
       </c>
       <c r="S23" s="12"/>
     </row>
-    <row r="24" spans="1:19" s="7" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:19" s="7" customFormat="1" ht="104.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>55</v>
@@ -2385,10 +2494,10 @@
         <v>186</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F24" s="18" t="s">
-        <v>192</v>
+        <v>184</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>183</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>24</v>
@@ -2399,8 +2508,8 @@
       <c r="I24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J24" s="1">
-        <v>2004</v>
+      <c r="J24" s="1" t="s">
+        <v>185</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>24</v>
@@ -2417,79 +2526,77 @@
       <c r="O24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="P24" s="1" t="s">
-        <v>193</v>
+      <c r="P24" s="14" t="s">
+        <v>187</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="R24" s="1" t="s">
         <v>30</v>
       </c>
       <c r="S24" s="12"/>
     </row>
-    <row r="25" spans="1:19" ht="40.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:19" s="7" customFormat="1" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>136</v>
+        <v>190</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>186</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>138</v>
+        <v>127</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>192</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="K25" s="1">
-        <v>5000</v>
-      </c>
-      <c r="L25" s="1">
-        <v>5000</v>
+        <v>24</v>
+      </c>
+      <c r="J25" s="1">
+        <v>2004</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>141</v>
+        <v>26</v>
       </c>
       <c r="N25" s="1" t="s">
         <v>27</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>142</v>
+        <v>24</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>143</v>
+        <v>193</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>144</v>
+        <v>191</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="S25" s="12" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" s="7" customFormat="1" ht="39" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="S25" s="12"/>
+    </row>
+    <row r="26" spans="1:19" ht="40.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>134</v>
@@ -2498,13 +2605,13 @@
         <v>135</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>137</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>24</v>
@@ -2513,10 +2620,10 @@
         <v>38</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="K26" s="1">
         <v>5000</v>
@@ -2546,9 +2653,9 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="52.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:19" s="7" customFormat="1" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>134</v>
@@ -2557,13 +2664,13 @@
         <v>135</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>137</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>24</v>
@@ -2572,10 +2679,10 @@
         <v>38</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="K27" s="1">
         <v>5000</v>
@@ -2605,646 +2712,648 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:19" s="7" customFormat="1" ht="26.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:19" ht="53.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="K28" s="1">
+        <v>5000</v>
+      </c>
+      <c r="L28" s="1">
+        <v>5000</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="R28" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="S28" s="12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" s="7" customFormat="1" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B29" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C29" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D29" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="E28" s="9" t="s">
+      <c r="E29" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F29" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G28" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H28" s="9" t="s">
+      <c r="G29" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H29" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="I28" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J28" s="9">
+      <c r="I29" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J29" s="9">
         <v>2020</v>
       </c>
-      <c r="K28" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="L28" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="M28" s="1" t="s">
+      <c r="K29" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="L29" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="M29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="N28" s="9" t="s">
+      <c r="N29" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="O28" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P28" s="14" t="s">
+      <c r="O29" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P29" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="Q28" s="5" t="s">
+      <c r="Q29" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="R28" s="9" t="s">
+      <c r="R29" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="S28" s="6"/>
-    </row>
-    <row r="29" spans="1:19" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="7" t="s">
+      <c r="S29" s="6"/>
+    </row>
+    <row r="30" spans="1:19" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B30" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C30" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D30" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="E30" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="F29" s="8" t="s">
+      <c r="F30" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="G29" s="10" t="s">
+      <c r="G30" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H29" s="10" t="s">
+      <c r="H30" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10">
+      <c r="I30" s="10"/>
+      <c r="J30" s="10">
         <v>2020</v>
       </c>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="7"/>
-      <c r="N29" s="10"/>
-      <c r="O29" s="10"/>
-      <c r="P29" s="7"/>
-      <c r="Q29" s="8"/>
-      <c r="R29" s="10"/>
-      <c r="S29" s="6"/>
-    </row>
-    <row r="30" spans="1:19" s="7" customFormat="1" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="8"/>
+      <c r="R30" s="10"/>
+      <c r="S30" s="6"/>
+    </row>
+    <row r="31" spans="1:19" s="7" customFormat="1" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B31" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C31" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D31" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="E30" s="9" t="s">
+      <c r="E31" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="F31" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="G30" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H30" s="9" t="s">
+      <c r="G31" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H31" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="I30" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J30" s="9">
+      <c r="I31" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J31" s="9">
         <v>2020</v>
       </c>
-      <c r="K30" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="L30" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="M30" s="1" t="s">
+      <c r="K31" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="L31" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="M31" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="N30" s="9" t="s">
+      <c r="N31" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="O30" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P30" s="14" t="s">
+      <c r="O31" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P31" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="Q30" s="5" t="s">
+      <c r="Q31" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="R30" s="9" t="s">
+      <c r="R31" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="S30" s="6"/>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A31" s="7" t="s">
+      <c r="S31" s="6"/>
+    </row>
+    <row r="32" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B32" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C32" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D32" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E32" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="F31" s="8" t="s">
+      <c r="F32" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="G31" s="10" t="s">
+      <c r="G32" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H31" s="10" t="s">
+      <c r="H32" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10">
+      <c r="I32" s="10"/>
+      <c r="J32" s="10">
         <v>2020</v>
       </c>
-      <c r="K31" s="10"/>
-      <c r="L31" s="10"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="10"/>
-      <c r="O31" s="10"/>
-      <c r="P31" s="7"/>
-      <c r="Q31" s="8"/>
-      <c r="R31" s="10"/>
-      <c r="S31" s="6"/>
-    </row>
-    <row r="32" spans="1:19" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="9" t="s">
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="10"/>
+      <c r="P32" s="7"/>
+      <c r="Q32" s="8"/>
+      <c r="R32" s="10"/>
+      <c r="S32" s="6"/>
+    </row>
+    <row r="33" spans="1:19" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B33" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C33" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="D33" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="E32" s="9" t="s">
+      <c r="E33" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F32" s="11" t="s">
+      <c r="F33" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="G32" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H32" s="9" t="s">
+      <c r="G33" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H33" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="I32" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J32" s="9">
+      <c r="I33" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J33" s="9">
         <v>2020</v>
       </c>
-      <c r="K32" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="L32" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="M32" s="1" t="s">
+      <c r="K33" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="L33" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="M33" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="N32" s="9" t="s">
+      <c r="N33" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="O32" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P32" s="14" t="s">
+      <c r="O33" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P33" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="Q32" s="9" t="s">
+      <c r="Q33" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="R32" s="9" t="s">
+      <c r="R33" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="S32" s="6" t="s">
+      <c r="S33" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="10" t="s">
+    <row r="34" spans="1:19" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B34" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C34" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D34" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="E33" s="10"/>
-      <c r="F33" s="8" t="s">
+      <c r="E34" s="10"/>
+      <c r="F34" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="G33" s="10" t="s">
+      <c r="G34" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H33" s="10" t="s">
+      <c r="H34" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10">
+      <c r="I34" s="10"/>
+      <c r="J34" s="10">
         <v>2020</v>
       </c>
-      <c r="K33" s="10"/>
-      <c r="L33" s="10"/>
-      <c r="M33" s="7"/>
-      <c r="N33" s="10"/>
-      <c r="O33" s="10"/>
-      <c r="P33" s="7"/>
-      <c r="Q33" s="10"/>
-      <c r="R33" s="10"/>
-      <c r="S33" s="6"/>
-    </row>
-    <row r="34" spans="1:19" s="7" customFormat="1" ht="26" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+      <c r="K34" s="10"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="10"/>
+      <c r="O34" s="10"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="10"/>
+      <c r="R34" s="10"/>
+      <c r="S34" s="6"/>
+    </row>
+    <row r="35" spans="1:19" s="7" customFormat="1" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B35" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C35" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="D35" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="E34" s="9" t="s">
+      <c r="E35" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="F35" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="G34" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H34" s="9" t="s">
+      <c r="G35" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H35" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="I34" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J34" s="9">
+      <c r="I35" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J35" s="9">
         <v>2020</v>
       </c>
-      <c r="K34" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="L34" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="M34" s="1" t="s">
+      <c r="K35" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="L35" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="M35" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="N34" s="9" t="s">
+      <c r="N35" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="O34" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P34" s="1" t="s">
+      <c r="O35" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P35" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="Q34" s="9" t="s">
+      <c r="Q35" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="R34" s="9" t="s">
+      <c r="R35" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="S34" s="6" t="s">
+      <c r="S35" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="7" t="s">
+    <row r="36" spans="1:19" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B36" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C36" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="D36" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E36" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="F35" s="8" t="s">
+      <c r="F36" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="G35" s="10" t="s">
+      <c r="G36" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H35" s="10" t="s">
+      <c r="H36" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="I35" s="10"/>
-      <c r="J35" s="10">
+      <c r="I36" s="10"/>
+      <c r="J36" s="10">
         <v>2020</v>
       </c>
-      <c r="K35" s="10"/>
-      <c r="L35" s="10"/>
-      <c r="M35" s="7"/>
-      <c r="N35" s="10"/>
-      <c r="O35" s="10"/>
-      <c r="P35" s="7"/>
-      <c r="Q35" s="10"/>
-      <c r="R35" s="10"/>
-      <c r="S35" s="6"/>
-    </row>
-    <row r="36" spans="1:19" s="7" customFormat="1" ht="26" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="10"/>
+      <c r="O36" s="10"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="10"/>
+      <c r="R36" s="10"/>
+      <c r="S36" s="6"/>
+    </row>
+    <row r="37" spans="1:19" s="7" customFormat="1" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B37" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C37" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D37" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="E36" s="9" t="s">
+      <c r="E37" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="F37" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="G36" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H36" s="9" t="s">
+      <c r="G37" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H37" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="I36" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J36" s="9">
+      <c r="I37" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J37" s="9">
         <v>2020</v>
       </c>
-      <c r="K36" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="L36" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="M36" s="1" t="s">
+      <c r="K37" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="L37" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="M37" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="N36" s="9" t="s">
+      <c r="N37" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="O36" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P36" s="1" t="s">
+      <c r="O37" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P37" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="Q36" s="9" t="s">
+      <c r="Q37" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="R36" s="9" t="s">
+      <c r="R37" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="S36" s="6" t="s">
+      <c r="S37" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A37" s="7" t="s">
+    <row r="38" spans="1:19" ht="27" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B38" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C38" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="D38" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E38" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="F37" s="8" t="s">
+      <c r="F38" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="G37" s="10" t="s">
+      <c r="G38" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H37" s="10" t="s">
+      <c r="H38" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="I37" s="10"/>
-      <c r="J37" s="10">
+      <c r="I38" s="10"/>
+      <c r="J38" s="10">
         <v>2020</v>
       </c>
-      <c r="K37" s="10"/>
-      <c r="L37" s="10"/>
-      <c r="M37" s="7"/>
-      <c r="N37" s="10"/>
-      <c r="O37" s="10"/>
-      <c r="P37" s="7"/>
-      <c r="Q37" s="10"/>
-      <c r="R37" s="10"/>
-      <c r="S37" s="13"/>
-    </row>
-    <row r="38" spans="1:19" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="1" t="s">
+      <c r="K38" s="10"/>
+      <c r="L38" s="10"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="10"/>
+      <c r="O38" s="10"/>
+      <c r="P38" s="7"/>
+      <c r="Q38" s="10"/>
+      <c r="R38" s="10"/>
+      <c r="S38" s="13"/>
+    </row>
+    <row r="39" spans="1:19" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B39" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C39" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D38" s="9" t="s">
+      <c r="D39" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="E38" s="9" t="s">
+      <c r="E39" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F38" s="5" t="s">
+      <c r="F39" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="G38" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H38" s="9" t="s">
+      <c r="G39" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H39" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="I38" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J38" s="9">
+      <c r="I39" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J39" s="9">
         <v>2020</v>
       </c>
-      <c r="K38" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="L38" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="M38" s="1" t="s">
+      <c r="K39" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="L39" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="M39" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="N38" s="9" t="s">
+      <c r="N39" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="O38" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P38" s="1" t="s">
+      <c r="O39" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P39" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Q38" s="5" t="s">
+      <c r="Q39" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="R38" s="9" t="s">
+      <c r="R39" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="S38" s="13"/>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A39" s="7" t="s">
+      <c r="S39" s="13"/>
+    </row>
+    <row r="40" spans="1:19" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B40" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C40" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="D40" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="E39" s="10" t="s">
+      <c r="E40" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="F39" s="8" t="s">
+      <c r="F40" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="G39" s="10" t="s">
+      <c r="G40" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H39" s="10" t="s">
+      <c r="H40" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10">
+      <c r="I40" s="10"/>
+      <c r="J40" s="10">
         <v>2020</v>
       </c>
-      <c r="K39" s="10"/>
-      <c r="L39" s="10"/>
-      <c r="M39" s="7"/>
-      <c r="N39" s="10"/>
-      <c r="O39" s="10"/>
-      <c r="P39" s="7"/>
-      <c r="Q39" s="8"/>
-      <c r="R39" s="10"/>
-      <c r="S39" s="13"/>
-    </row>
-    <row r="40" spans="1:19" ht="39.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="1" t="s">
+      <c r="K40" s="10"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="10"/>
+      <c r="O40" s="10"/>
+      <c r="P40" s="7"/>
+      <c r="Q40" s="8"/>
+      <c r="R40" s="10"/>
+      <c r="S40" s="13"/>
+    </row>
+    <row r="41" spans="1:19" ht="39" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="G40" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H40" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="I40" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J40" s="9">
-        <v>2020</v>
-      </c>
-      <c r="K40" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="L40" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="M40" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N40" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="O40" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P40" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q40" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="R40" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="S40" s="13"/>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A41" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="B41" s="9" t="s">
         <v>83</v>
@@ -3253,46 +3362,104 @@
         <v>20</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E41" s="9" t="s">
         <v>46</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="H41" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="I41" s="9"/>
+        <v>43</v>
+      </c>
+      <c r="I41" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="J41" s="9">
         <v>2020</v>
       </c>
-      <c r="K41" s="9"/>
-      <c r="L41" s="9"/>
-      <c r="N41" s="9"/>
-      <c r="O41" s="9"/>
-      <c r="Q41" s="5"/>
-      <c r="R41" s="9"/>
+      <c r="K41" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="L41" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N41" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="O41" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P41" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q41" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="R41" s="9" t="s">
+        <v>30</v>
+      </c>
       <c r="S41" s="13"/>
     </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H42" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9">
+        <v>2020</v>
+      </c>
+      <c r="K42" s="9"/>
+      <c r="L42" s="9"/>
+      <c r="N42" s="9"/>
+      <c r="O42" s="9"/>
+      <c r="Q42" s="5"/>
+      <c r="R42" s="9"/>
+      <c r="S42" s="13"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:S5">
-    <sortState ref="A2:S33">
+  <autoFilter ref="A1:S5" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S33">
       <sortCondition ref="B1:B5"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="P28" r:id="rId1"/>
-    <hyperlink ref="P32" r:id="rId2"/>
-    <hyperlink ref="P30" r:id="rId3"/>
-    <hyperlink ref="P40" r:id="rId4"/>
-    <hyperlink ref="P19" r:id="rId5"/>
+    <hyperlink ref="P29" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="P33" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="P31" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="P41" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="P19" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="P20" r:id="rId6" display="https://www.lantmateriet.se/sv/Om-Lantmateriet/Samverkan-med-andra/internationell-samverkan/corine-land-cover/" xr:uid="{6B959786-6DFA-4235-BB04-24C8BD502CA4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added updated os scripts to build PostGIS and GRASS databases, working on them yet
</commit_message>
<xml_diff>
--- a/data/spatialdb_metadata_sweden_20211101.xlsx
+++ b/data/spatialdb_metadata_sweden_20211101.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\41203800_oneimpact\grass-db\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E293B8-647A-4744-B79E-2B3825E97B0C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FB3456-C5FB-424C-8BB5-BEE5E76082A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1225,9 +1225,9 @@
   <dimension ref="A1:TW42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="S42" sqref="A1:S42"/>
+      <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>